<commit_message>
Setting up for regression modelling
</commit_message>
<xml_diff>
--- a/data_and_preprocessing/feature_rework.xlsx
+++ b/data_and_preprocessing/feature_rework.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dann/Desktop/AI-Project-Toronto-Major-Crime-Indicators/data_and_preprocessing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siosonda\Desktop\AI-Project-Toronto-Major-Crime-Indicators\data_and_preprocessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F85A8B-A81D-654E-8212-ABFBCDFAC2F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16940" activeTab="3" xr2:uid="{7A66232D-3EAE-8241-85BD-217EEA64247F}"/>
+    <workbookView xWindow="1500" yWindow="2520" windowWidth="27640" windowHeight="16940" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LOCATION_TYPE" sheetId="1" r:id="rId1"/>
@@ -18,13 +17,14 @@
     <sheet name="OFFENCE" sheetId="3" r:id="rId3"/>
     <sheet name="MONTH" sheetId="4" r:id="rId4"/>
     <sheet name="DAY" sheetId="5" r:id="rId5"/>
+    <sheet name="HOLIDAYS" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LOCATION_TYPE!$A$1:$C$55</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">OFFENCE!$A$1:$C$52</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">UCR_CODE!$A$1:$D$23</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="180">
   <si>
     <t>LOCATION_TYPE</t>
   </si>
@@ -302,9 +302,6 @@
     <t>Assaults</t>
   </si>
   <si>
-    <t>Other Violations Involving Violence or The Threat of Voilence</t>
-  </si>
-  <si>
     <t>Property Crimes</t>
   </si>
   <si>
@@ -540,13 +537,61 @@
   </si>
   <si>
     <t>DOW_NUM</t>
+  </si>
+  <si>
+    <t>YEAR</t>
+  </si>
+  <si>
+    <t>DAY</t>
+  </si>
+  <si>
+    <t>IS_HOLIDAY</t>
+  </si>
+  <si>
+    <t>HOLIDAY_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>New Years</t>
+  </si>
+  <si>
+    <t>Family Day</t>
+  </si>
+  <si>
+    <t>Good Friday</t>
+  </si>
+  <si>
+    <t>Victoria Day</t>
+  </si>
+  <si>
+    <t>Canada Day</t>
+  </si>
+  <si>
+    <t>Civic Holiday</t>
+  </si>
+  <si>
+    <t>Labour Day</t>
+  </si>
+  <si>
+    <t>Thanksgiving</t>
+  </si>
+  <si>
+    <t>Christmas</t>
+  </si>
+  <si>
+    <t>Boxing Day</t>
+  </si>
+  <si>
+    <t>Other Violations Involving Violence or The Threat of Violence</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -916,20 +961,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BD2E716-9C54-B545-880B-62BDFB6A26D1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="60.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="60.5" customWidth="1"/>
+    <col min="1" max="1" width="60.4609375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.4609375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -940,7 +985,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -951,7 +996,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -962,7 +1007,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -973,7 +1018,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -984,7 +1029,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -995,7 +1040,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -1006,7 +1051,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -1017,7 +1062,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -1028,7 +1073,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -1039,7 +1084,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>52</v>
       </c>
@@ -1050,7 +1095,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -1061,7 +1106,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -1072,7 +1117,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -1083,7 +1128,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -1094,7 +1139,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1105,7 +1150,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -1116,7 +1161,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -1127,7 +1172,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -1138,7 +1183,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -1149,7 +1194,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -1160,7 +1205,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -1171,7 +1216,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -1182,7 +1227,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1193,7 +1238,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -1204,7 +1249,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -1215,7 +1260,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>50</v>
       </c>
@@ -1226,7 +1271,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1237,7 +1282,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -1248,7 +1293,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -1259,7 +1304,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>49</v>
       </c>
@@ -1270,7 +1315,7 @@
         <v>1205</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
         <v>8</v>
       </c>
@@ -1281,7 +1326,7 @@
         <v>1292</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
         <v>21</v>
       </c>
@@ -1292,7 +1337,7 @@
         <v>1439</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>31</v>
       </c>
@@ -1303,7 +1348,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -1314,7 +1359,7 @@
         <v>2063</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
         <v>20</v>
       </c>
@@ -1325,7 +1370,7 @@
         <v>2192</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3">
       <c r="A37" t="s">
         <v>22</v>
       </c>
@@ -1336,7 +1381,7 @@
         <v>2553</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
         <v>26</v>
       </c>
@@ -1347,7 +1392,7 @@
         <v>2618</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
         <v>19</v>
       </c>
@@ -1358,7 +1403,7 @@
         <v>2774</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3">
       <c r="A40" t="s">
         <v>15</v>
       </c>
@@ -1369,7 +1414,7 @@
         <v>3214</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3">
       <c r="A41" t="s">
         <v>25</v>
       </c>
@@ -1380,7 +1425,7 @@
         <v>3330</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3">
       <c r="A42" t="s">
         <v>13</v>
       </c>
@@ -1391,7 +1436,7 @@
         <v>3392</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
         <v>28</v>
       </c>
@@ -1402,7 +1447,7 @@
         <v>3450</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3">
       <c r="A44" t="s">
         <v>23</v>
       </c>
@@ -1413,7 +1458,7 @@
         <v>4063</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3">
       <c r="A45" t="s">
         <v>6</v>
       </c>
@@ -1424,7 +1469,7 @@
         <v>4336</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3">
       <c r="A46" t="s">
         <v>18</v>
       </c>
@@ -1435,7 +1480,7 @@
         <v>5065</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3">
       <c r="A47" t="s">
         <v>7</v>
       </c>
@@ -1446,7 +1491,7 @@
         <v>5170</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3">
       <c r="A48" t="s">
         <v>16</v>
       </c>
@@ -1457,7 +1502,7 @@
         <v>5922</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3">
       <c r="A49" t="s">
         <v>11</v>
       </c>
@@ -1468,7 +1513,7 @@
         <v>7847</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3">
       <c r="A50" t="s">
         <v>5</v>
       </c>
@@ -1479,7 +1524,7 @@
         <v>15061</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3">
       <c r="A51" t="s">
         <v>10</v>
       </c>
@@ -1490,7 +1535,7 @@
         <v>36385</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3">
       <c r="A52" t="s">
         <v>2</v>
       </c>
@@ -1501,7 +1546,7 @@
         <v>45520</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3">
       <c r="A53" t="s">
         <v>3</v>
       </c>
@@ -1512,7 +1557,7 @@
         <v>61438</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3">
       <c r="A54" t="s">
         <v>4</v>
       </c>
@@ -1523,7 +1568,7 @@
         <v>72168</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3">
       <c r="A55" t="s">
         <v>1</v>
       </c>
@@ -1535,8 +1580,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C55" xr:uid="{7BD2E716-9C54-B545-880B-62BDFB6A26D1}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C55">
+  <autoFilter ref="A1:C55">
+    <sortState ref="A2:C55">
       <sortCondition ref="C1:C55"/>
     </sortState>
   </autoFilter>
@@ -1545,19 +1590,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D2ED7AE-0B89-D047-A53F-C803DDD548E8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" customWidth="1"/>
+    <col min="1" max="1" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -1571,7 +1616,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1410</v>
       </c>
@@ -1585,7 +1630,7 @@
         <v>3003</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>1420</v>
       </c>
@@ -1599,7 +1644,7 @@
         <v>45035</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>1430</v>
       </c>
@@ -1613,7 +1658,7 @@
         <v>144548</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>1440</v>
       </c>
@@ -1627,7 +1672,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>1450</v>
       </c>
@@ -1641,7 +1686,7 @@
         <v>4236</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>1455</v>
       </c>
@@ -1655,7 +1700,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>1457</v>
       </c>
@@ -1669,7 +1714,7 @@
         <v>1424</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>1460</v>
       </c>
@@ -1683,7 +1728,7 @@
         <v>6788</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>1461</v>
       </c>
@@ -1697,7 +1742,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>1462</v>
       </c>
@@ -1711,7 +1756,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>1470</v>
       </c>
@@ -1725,7 +1770,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>1475</v>
       </c>
@@ -1739,7 +1784,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>1480</v>
       </c>
@@ -1753,7 +1798,7 @@
         <v>4222</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>1610</v>
       </c>
@@ -1761,13 +1806,13 @@
         <v>72</v>
       </c>
       <c r="C15" t="s">
-        <v>85</v>
+        <v>179</v>
       </c>
       <c r="D15">
         <v>35572</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="A16">
         <v>1611</v>
       </c>
@@ -1775,13 +1820,13 @@
         <v>73</v>
       </c>
       <c r="C16" t="s">
-        <v>85</v>
+        <v>179</v>
       </c>
       <c r="D16">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>2120</v>
       </c>
@@ -1789,13 +1834,13 @@
         <v>74</v>
       </c>
       <c r="C17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D17">
         <v>73669</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>2121</v>
       </c>
@@ -1803,13 +1848,13 @@
         <v>75</v>
       </c>
       <c r="C18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D18">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>2125</v>
       </c>
@@ -1817,13 +1862,13 @@
         <v>78</v>
       </c>
       <c r="C19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D19">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>2130</v>
       </c>
@@ -1831,13 +1876,13 @@
         <v>76</v>
       </c>
       <c r="C20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D20">
         <v>9446</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>2132</v>
       </c>
@@ -1845,13 +1890,13 @@
         <v>79</v>
       </c>
       <c r="C21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D21">
         <v>3278</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>2133</v>
       </c>
@@ -1859,13 +1904,13 @@
         <v>80</v>
       </c>
       <c r="C22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D22">
         <v>664</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>2135</v>
       </c>
@@ -1873,15 +1918,15 @@
         <v>81</v>
       </c>
       <c r="C23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D23">
         <v>63633</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D23" xr:uid="{9D2ED7AE-0B89-D047-A53F-C803DDD548E8}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D23">
+  <autoFilter ref="A1:D23">
+    <sortState ref="A2:D23">
       <sortCondition ref="A1:A23"/>
     </sortState>
   </autoFilter>
@@ -1890,163 +1935,163 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F48C0619-F73D-8041-BAC1-0121D3A208A9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" customWidth="1"/>
+    <col min="1" max="1" width="27.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.3046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C2">
         <v>657</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C3">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C4">
         <v>2984</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C5">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C6">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>83</v>
       </c>
       <c r="B7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C7">
         <v>144101</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C8">
         <v>447</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C9">
         <v>3563</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C10">
         <v>9090</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C11">
         <v>6655</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C12">
         <v>785</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C13">
         <v>35945</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B14" t="s">
         <v>74</v>
@@ -2055,9 +2100,9 @@
         <v>61954</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B15" t="s">
         <v>74</v>
@@ -2066,9 +2111,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B16" t="s">
         <v>74</v>
@@ -2077,9 +2122,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B17" t="s">
         <v>74</v>
@@ -2088,9 +2133,9 @@
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B18" t="s">
         <v>74</v>
@@ -2099,75 +2144,75 @@
         <v>9249</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C19">
         <v>133</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C20">
         <v>133</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C21">
         <v>1763</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C22">
         <v>2442</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C24">
         <v>1424</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B25" t="s">
         <v>72</v>
@@ -2176,9 +2221,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B26" t="s">
         <v>72</v>
@@ -2187,9 +2232,9 @@
         <v>119</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B27" t="s">
         <v>72</v>
@@ -2198,9 +2243,9 @@
         <v>5424</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B28" t="s">
         <v>72</v>
@@ -2209,9 +2254,9 @@
         <v>313</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B29" t="s">
         <v>72</v>
@@ -2220,9 +2265,9 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B30" t="s">
         <v>72</v>
@@ -2231,9 +2276,9 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B31" t="s">
         <v>72</v>
@@ -2242,9 +2287,9 @@
         <v>9257</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B32" t="s">
         <v>72</v>
@@ -2253,9 +2298,9 @@
         <v>5922</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B33" t="s">
         <v>72</v>
@@ -2264,9 +2309,9 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B34" t="s">
         <v>72</v>
@@ -2275,9 +2320,9 @@
         <v>2622</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B35" t="s">
         <v>72</v>
@@ -2286,9 +2331,9 @@
         <v>269</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B36" t="s">
         <v>72</v>
@@ -2297,9 +2342,9 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B37" t="s">
         <v>72</v>
@@ -2308,9 +2353,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B38" t="s">
         <v>72</v>
@@ -2319,141 +2364,141 @@
         <v>6605</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B39" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C39">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B40" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C40">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B41" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C41">
         <v>1530</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B42" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C42">
         <v>3278</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B43" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C43">
         <v>63633</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B44" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C44">
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B45" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C45">
         <v>7516</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B46" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C46">
         <v>193</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B47" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C47">
         <v>159</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B48" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C48">
         <v>664</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B49" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C49">
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3">
       <c r="A50" t="s">
         <v>62</v>
       </c>
       <c r="B50" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C50">
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B51" t="s">
         <v>74</v>
@@ -2462,20 +2507,20 @@
         <v>2349</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B52" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C52">
         <v>219</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C52" xr:uid="{F48C0619-F73D-8041-BAC1-0121D3A208A9}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C52">
+  <autoFilter ref="A1:C52">
+    <sortState ref="A2:C52">
       <sortCondition ref="A1:A52"/>
     </sortState>
   </autoFilter>
@@ -2484,112 +2529,112 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3F542BC-B0AA-424F-A70C-9E649335C0AE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15.5"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" t="s">
         <v>142</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
         <v>143</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>144</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -2602,72 +2647,72 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99CDB83A-1029-054A-A806-449C65B859A7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15.5"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" t="s">
         <v>163</v>
       </c>
-      <c r="B1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -2677,4 +2722,1564 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E91"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>2018</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>2018</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>2018</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
+        <v>168</v>
+      </c>
+      <c r="E4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>2018</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>2018</v>
+      </c>
+      <c r="B6">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>168</v>
+      </c>
+      <c r="E6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>2018</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>168</v>
+      </c>
+      <c r="E7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>2018</v>
+      </c>
+      <c r="B8">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>168</v>
+      </c>
+      <c r="E8" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>2018</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E9" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>2018</v>
+      </c>
+      <c r="B10">
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>168</v>
+      </c>
+      <c r="E10" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>2018</v>
+      </c>
+      <c r="B11">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>168</v>
+      </c>
+      <c r="E11" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>2019</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>168</v>
+      </c>
+      <c r="E12" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>2019</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>18</v>
+      </c>
+      <c r="D13" t="s">
+        <v>168</v>
+      </c>
+      <c r="E13" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>2019</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>19</v>
+      </c>
+      <c r="D14" t="s">
+        <v>168</v>
+      </c>
+      <c r="E14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15">
+        <v>2019</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>20</v>
+      </c>
+      <c r="D15" t="s">
+        <v>168</v>
+      </c>
+      <c r="E15" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16">
+        <v>2019</v>
+      </c>
+      <c r="B16">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>168</v>
+      </c>
+      <c r="E16" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>2019</v>
+      </c>
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>168</v>
+      </c>
+      <c r="E17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>2019</v>
+      </c>
+      <c r="B18">
+        <v>9</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>168</v>
+      </c>
+      <c r="E18" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>2019</v>
+      </c>
+      <c r="B19">
+        <v>10</v>
+      </c>
+      <c r="C19">
+        <v>14</v>
+      </c>
+      <c r="D19" t="s">
+        <v>168</v>
+      </c>
+      <c r="E19" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20">
+        <v>2019</v>
+      </c>
+      <c r="B20">
+        <v>12</v>
+      </c>
+      <c r="C20">
+        <v>25</v>
+      </c>
+      <c r="D20" t="s">
+        <v>168</v>
+      </c>
+      <c r="E20" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21">
+        <v>2019</v>
+      </c>
+      <c r="B21">
+        <v>12</v>
+      </c>
+      <c r="C21">
+        <v>26</v>
+      </c>
+      <c r="D21" t="s">
+        <v>168</v>
+      </c>
+      <c r="E21" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22">
+        <v>2020</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>168</v>
+      </c>
+      <c r="E22" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23">
+        <v>2020</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>17</v>
+      </c>
+      <c r="D23" t="s">
+        <v>168</v>
+      </c>
+      <c r="E23" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24">
+        <v>2020</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>10</v>
+      </c>
+      <c r="D24" t="s">
+        <v>168</v>
+      </c>
+      <c r="E24" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25">
+        <v>2020</v>
+      </c>
+      <c r="B25">
+        <v>5</v>
+      </c>
+      <c r="C25">
+        <v>18</v>
+      </c>
+      <c r="D25" t="s">
+        <v>168</v>
+      </c>
+      <c r="E25" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26">
+        <v>2020</v>
+      </c>
+      <c r="B26">
+        <v>7</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>168</v>
+      </c>
+      <c r="E26" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27">
+        <v>2020</v>
+      </c>
+      <c r="B27">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>168</v>
+      </c>
+      <c r="E27" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28">
+        <v>2020</v>
+      </c>
+      <c r="B28">
+        <v>9</v>
+      </c>
+      <c r="C28">
+        <v>7</v>
+      </c>
+      <c r="D28" t="s">
+        <v>168</v>
+      </c>
+      <c r="E28" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29">
+        <v>2020</v>
+      </c>
+      <c r="B29">
+        <v>10</v>
+      </c>
+      <c r="C29">
+        <v>12</v>
+      </c>
+      <c r="D29" t="s">
+        <v>168</v>
+      </c>
+      <c r="E29" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30">
+        <v>2020</v>
+      </c>
+      <c r="B30">
+        <v>12</v>
+      </c>
+      <c r="C30">
+        <v>25</v>
+      </c>
+      <c r="D30" t="s">
+        <v>168</v>
+      </c>
+      <c r="E30" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31">
+        <v>2020</v>
+      </c>
+      <c r="B31">
+        <v>12</v>
+      </c>
+      <c r="C31">
+        <v>26</v>
+      </c>
+      <c r="D31" t="s">
+        <v>168</v>
+      </c>
+      <c r="E31" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32">
+        <v>2021</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>168</v>
+      </c>
+      <c r="E32" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33">
+        <v>2021</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33">
+        <v>15</v>
+      </c>
+      <c r="D33" t="s">
+        <v>168</v>
+      </c>
+      <c r="E33" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34">
+        <v>2021</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>168</v>
+      </c>
+      <c r="E34" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35">
+        <v>2021</v>
+      </c>
+      <c r="B35">
+        <v>5</v>
+      </c>
+      <c r="C35">
+        <v>24</v>
+      </c>
+      <c r="D35" t="s">
+        <v>168</v>
+      </c>
+      <c r="E35" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36">
+        <v>2021</v>
+      </c>
+      <c r="B36">
+        <v>7</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36" t="s">
+        <v>168</v>
+      </c>
+      <c r="E36" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37">
+        <v>2021</v>
+      </c>
+      <c r="B37">
+        <v>8</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37" t="s">
+        <v>168</v>
+      </c>
+      <c r="E37" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38">
+        <v>2021</v>
+      </c>
+      <c r="B38">
+        <v>9</v>
+      </c>
+      <c r="C38">
+        <v>6</v>
+      </c>
+      <c r="D38" t="s">
+        <v>168</v>
+      </c>
+      <c r="E38" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39">
+        <v>2021</v>
+      </c>
+      <c r="B39">
+        <v>10</v>
+      </c>
+      <c r="C39">
+        <v>11</v>
+      </c>
+      <c r="D39" t="s">
+        <v>168</v>
+      </c>
+      <c r="E39" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40">
+        <v>2021</v>
+      </c>
+      <c r="B40">
+        <v>12</v>
+      </c>
+      <c r="C40">
+        <v>25</v>
+      </c>
+      <c r="D40" t="s">
+        <v>168</v>
+      </c>
+      <c r="E40" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41">
+        <v>2021</v>
+      </c>
+      <c r="B41">
+        <v>12</v>
+      </c>
+      <c r="C41">
+        <v>26</v>
+      </c>
+      <c r="D41" t="s">
+        <v>168</v>
+      </c>
+      <c r="E41" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42">
+        <v>2022</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42" t="s">
+        <v>168</v>
+      </c>
+      <c r="E42" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43">
+        <v>2022</v>
+      </c>
+      <c r="B43">
+        <v>2</v>
+      </c>
+      <c r="C43">
+        <v>21</v>
+      </c>
+      <c r="D43" t="s">
+        <v>168</v>
+      </c>
+      <c r="E43" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44">
+        <v>2022</v>
+      </c>
+      <c r="B44">
+        <v>4</v>
+      </c>
+      <c r="C44">
+        <v>15</v>
+      </c>
+      <c r="D44" t="s">
+        <v>168</v>
+      </c>
+      <c r="E44" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45">
+        <v>2022</v>
+      </c>
+      <c r="B45">
+        <v>5</v>
+      </c>
+      <c r="C45">
+        <v>23</v>
+      </c>
+      <c r="D45" t="s">
+        <v>168</v>
+      </c>
+      <c r="E45" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46">
+        <v>2022</v>
+      </c>
+      <c r="B46">
+        <v>7</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46" t="s">
+        <v>168</v>
+      </c>
+      <c r="E46" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47">
+        <v>2022</v>
+      </c>
+      <c r="B47">
+        <v>8</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47" t="s">
+        <v>168</v>
+      </c>
+      <c r="E47" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48">
+        <v>2022</v>
+      </c>
+      <c r="B48">
+        <v>9</v>
+      </c>
+      <c r="C48">
+        <v>5</v>
+      </c>
+      <c r="D48" t="s">
+        <v>168</v>
+      </c>
+      <c r="E48" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49">
+        <v>2022</v>
+      </c>
+      <c r="B49">
+        <v>10</v>
+      </c>
+      <c r="C49">
+        <v>10</v>
+      </c>
+      <c r="D49" t="s">
+        <v>168</v>
+      </c>
+      <c r="E49" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50">
+        <v>2022</v>
+      </c>
+      <c r="B50">
+        <v>12</v>
+      </c>
+      <c r="C50">
+        <v>25</v>
+      </c>
+      <c r="D50" t="s">
+        <v>168</v>
+      </c>
+      <c r="E50" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51">
+        <v>2022</v>
+      </c>
+      <c r="B51">
+        <v>12</v>
+      </c>
+      <c r="C51">
+        <v>26</v>
+      </c>
+      <c r="D51" t="s">
+        <v>168</v>
+      </c>
+      <c r="E51" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52">
+        <v>2023</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52" t="s">
+        <v>168</v>
+      </c>
+      <c r="E52" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53">
+        <v>2024</v>
+      </c>
+      <c r="B53">
+        <v>2</v>
+      </c>
+      <c r="C53">
+        <v>20</v>
+      </c>
+      <c r="D53" t="s">
+        <v>168</v>
+      </c>
+      <c r="E53" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54">
+        <v>2024</v>
+      </c>
+      <c r="B54">
+        <v>4</v>
+      </c>
+      <c r="C54">
+        <v>7</v>
+      </c>
+      <c r="D54" t="s">
+        <v>168</v>
+      </c>
+      <c r="E54" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55">
+        <v>2024</v>
+      </c>
+      <c r="B55">
+        <v>5</v>
+      </c>
+      <c r="C55">
+        <v>22</v>
+      </c>
+      <c r="D55" t="s">
+        <v>168</v>
+      </c>
+      <c r="E55" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56">
+        <v>2024</v>
+      </c>
+      <c r="B56">
+        <v>7</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56" t="s">
+        <v>168</v>
+      </c>
+      <c r="E56" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57">
+        <v>2024</v>
+      </c>
+      <c r="B57">
+        <v>8</v>
+      </c>
+      <c r="C57">
+        <v>7</v>
+      </c>
+      <c r="D57" t="s">
+        <v>168</v>
+      </c>
+      <c r="E57" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58">
+        <v>2024</v>
+      </c>
+      <c r="B58">
+        <v>9</v>
+      </c>
+      <c r="C58">
+        <v>4</v>
+      </c>
+      <c r="D58" t="s">
+        <v>168</v>
+      </c>
+      <c r="E58" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59">
+        <v>2024</v>
+      </c>
+      <c r="B59">
+        <v>10</v>
+      </c>
+      <c r="C59">
+        <v>9</v>
+      </c>
+      <c r="D59" t="s">
+        <v>168</v>
+      </c>
+      <c r="E59" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60">
+        <v>2024</v>
+      </c>
+      <c r="B60">
+        <v>12</v>
+      </c>
+      <c r="C60">
+        <v>25</v>
+      </c>
+      <c r="D60" t="s">
+        <v>168</v>
+      </c>
+      <c r="E60" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61">
+        <v>2024</v>
+      </c>
+      <c r="B61">
+        <v>12</v>
+      </c>
+      <c r="C61">
+        <v>26</v>
+      </c>
+      <c r="D61" t="s">
+        <v>168</v>
+      </c>
+      <c r="E61" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62">
+        <v>2025</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62" t="s">
+        <v>168</v>
+      </c>
+      <c r="E62" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63">
+        <v>2025</v>
+      </c>
+      <c r="B63">
+        <v>2</v>
+      </c>
+      <c r="C63">
+        <v>17</v>
+      </c>
+      <c r="D63" t="s">
+        <v>168</v>
+      </c>
+      <c r="E63" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64">
+        <v>2025</v>
+      </c>
+      <c r="B64">
+        <v>4</v>
+      </c>
+      <c r="C64">
+        <v>18</v>
+      </c>
+      <c r="D64" t="s">
+        <v>168</v>
+      </c>
+      <c r="E64" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65">
+        <v>2025</v>
+      </c>
+      <c r="B65">
+        <v>5</v>
+      </c>
+      <c r="C65">
+        <v>19</v>
+      </c>
+      <c r="D65" t="s">
+        <v>168</v>
+      </c>
+      <c r="E65" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66">
+        <v>2025</v>
+      </c>
+      <c r="B66">
+        <v>7</v>
+      </c>
+      <c r="C66">
+        <v>1</v>
+      </c>
+      <c r="D66" t="s">
+        <v>168</v>
+      </c>
+      <c r="E66" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67">
+        <v>2025</v>
+      </c>
+      <c r="B67">
+        <v>8</v>
+      </c>
+      <c r="C67">
+        <v>4</v>
+      </c>
+      <c r="D67" t="s">
+        <v>168</v>
+      </c>
+      <c r="E67" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68">
+        <v>2025</v>
+      </c>
+      <c r="B68">
+        <v>9</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68" t="s">
+        <v>168</v>
+      </c>
+      <c r="E68" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69">
+        <v>2025</v>
+      </c>
+      <c r="B69">
+        <v>10</v>
+      </c>
+      <c r="C69">
+        <v>13</v>
+      </c>
+      <c r="D69" t="s">
+        <v>168</v>
+      </c>
+      <c r="E69" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70">
+        <v>2025</v>
+      </c>
+      <c r="B70">
+        <v>12</v>
+      </c>
+      <c r="C70">
+        <v>25</v>
+      </c>
+      <c r="D70" t="s">
+        <v>168</v>
+      </c>
+      <c r="E70" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71">
+        <v>2025</v>
+      </c>
+      <c r="B71">
+        <v>12</v>
+      </c>
+      <c r="C71">
+        <v>26</v>
+      </c>
+      <c r="D71" t="s">
+        <v>168</v>
+      </c>
+      <c r="E71" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72">
+        <v>2026</v>
+      </c>
+      <c r="B72">
+        <v>1</v>
+      </c>
+      <c r="C72">
+        <v>1</v>
+      </c>
+      <c r="D72" t="s">
+        <v>168</v>
+      </c>
+      <c r="E72" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73">
+        <v>2026</v>
+      </c>
+      <c r="B73">
+        <v>2</v>
+      </c>
+      <c r="C73">
+        <v>16</v>
+      </c>
+      <c r="D73" t="s">
+        <v>168</v>
+      </c>
+      <c r="E73" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74">
+        <v>2026</v>
+      </c>
+      <c r="B74">
+        <v>4</v>
+      </c>
+      <c r="C74">
+        <v>3</v>
+      </c>
+      <c r="D74" t="s">
+        <v>168</v>
+      </c>
+      <c r="E74" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75">
+        <v>2026</v>
+      </c>
+      <c r="B75">
+        <v>5</v>
+      </c>
+      <c r="C75">
+        <v>18</v>
+      </c>
+      <c r="D75" t="s">
+        <v>168</v>
+      </c>
+      <c r="E75" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76">
+        <v>2026</v>
+      </c>
+      <c r="B76">
+        <v>7</v>
+      </c>
+      <c r="C76">
+        <v>1</v>
+      </c>
+      <c r="D76" t="s">
+        <v>168</v>
+      </c>
+      <c r="E76" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77">
+        <v>2026</v>
+      </c>
+      <c r="B77">
+        <v>8</v>
+      </c>
+      <c r="C77">
+        <v>3</v>
+      </c>
+      <c r="D77" t="s">
+        <v>168</v>
+      </c>
+      <c r="E77" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78">
+        <v>2026</v>
+      </c>
+      <c r="B78">
+        <v>9</v>
+      </c>
+      <c r="C78">
+        <v>7</v>
+      </c>
+      <c r="D78" t="s">
+        <v>168</v>
+      </c>
+      <c r="E78" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79">
+        <v>2026</v>
+      </c>
+      <c r="B79">
+        <v>10</v>
+      </c>
+      <c r="C79">
+        <v>12</v>
+      </c>
+      <c r="D79" t="s">
+        <v>168</v>
+      </c>
+      <c r="E79" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80">
+        <v>2026</v>
+      </c>
+      <c r="B80">
+        <v>12</v>
+      </c>
+      <c r="C80">
+        <v>25</v>
+      </c>
+      <c r="D80" t="s">
+        <v>168</v>
+      </c>
+      <c r="E80" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81">
+        <v>2026</v>
+      </c>
+      <c r="B81">
+        <v>12</v>
+      </c>
+      <c r="C81">
+        <v>26</v>
+      </c>
+      <c r="D81" t="s">
+        <v>168</v>
+      </c>
+      <c r="E81" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82">
+        <v>2027</v>
+      </c>
+      <c r="B82">
+        <v>1</v>
+      </c>
+      <c r="C82">
+        <v>1</v>
+      </c>
+      <c r="D82" t="s">
+        <v>168</v>
+      </c>
+      <c r="E82" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83">
+        <v>2027</v>
+      </c>
+      <c r="B83">
+        <v>2</v>
+      </c>
+      <c r="C83">
+        <v>15</v>
+      </c>
+      <c r="D83" t="s">
+        <v>168</v>
+      </c>
+      <c r="E83" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84">
+        <v>2027</v>
+      </c>
+      <c r="B84">
+        <v>3</v>
+      </c>
+      <c r="C84">
+        <v>26</v>
+      </c>
+      <c r="D84" t="s">
+        <v>168</v>
+      </c>
+      <c r="E84" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85">
+        <v>2027</v>
+      </c>
+      <c r="B85">
+        <v>5</v>
+      </c>
+      <c r="C85">
+        <v>24</v>
+      </c>
+      <c r="D85" t="s">
+        <v>168</v>
+      </c>
+      <c r="E85" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86">
+        <v>2027</v>
+      </c>
+      <c r="B86">
+        <v>7</v>
+      </c>
+      <c r="C86">
+        <v>1</v>
+      </c>
+      <c r="D86" t="s">
+        <v>168</v>
+      </c>
+      <c r="E86" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87">
+        <v>2027</v>
+      </c>
+      <c r="B87">
+        <v>8</v>
+      </c>
+      <c r="C87">
+        <v>2</v>
+      </c>
+      <c r="D87" t="s">
+        <v>168</v>
+      </c>
+      <c r="E87" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88">
+        <v>2027</v>
+      </c>
+      <c r="B88">
+        <v>9</v>
+      </c>
+      <c r="C88">
+        <v>6</v>
+      </c>
+      <c r="D88" t="s">
+        <v>168</v>
+      </c>
+      <c r="E88" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89">
+        <v>2027</v>
+      </c>
+      <c r="B89">
+        <v>10</v>
+      </c>
+      <c r="C89">
+        <v>11</v>
+      </c>
+      <c r="D89" t="s">
+        <v>168</v>
+      </c>
+      <c r="E89" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90">
+        <v>2027</v>
+      </c>
+      <c r="B90">
+        <v>12</v>
+      </c>
+      <c r="C90">
+        <v>25</v>
+      </c>
+      <c r="D90" t="s">
+        <v>168</v>
+      </c>
+      <c r="E90" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91">
+        <v>2027</v>
+      </c>
+      <c r="B91">
+        <v>12</v>
+      </c>
+      <c r="C91">
+        <v>26</v>
+      </c>
+      <c r="D91" t="s">
+        <v>168</v>
+      </c>
+      <c r="E91" t="s">
+        <v>178</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>